<commit_message>
New script for extracting party/geo affiliations for committees
</commit_message>
<xml_diff>
--- a/tests/directory.xlsx
+++ b/tests/directory.xlsx
@@ -1,61 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sean\OneDrive\Tufts Daily\fec-donation-aggregator\tests\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="11_4D7842D3F8281A2758868A22BC512389E1A5535A" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{0FFCB712-E262-4219-974D-66087ECEDB63}"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible" windowHeight="15840" windowWidth="29040" xWindow="-120" yWindow="-120"/>
   </bookViews>
   <sheets>
-    <sheet name="DirectoryResults" sheetId="1" r:id="rId1"/>
+    <sheet name="DirectoryResults" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <definedNames/>
+  <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
-  <si>
-    <t>full_name</t>
-  </si>
-  <si>
-    <t>directory_result</t>
-  </si>
-  <si>
-    <t>ABOWD, THOMAS</t>
-  </si>
-  <si>
-    <t>ABRAMS, DANIELLE</t>
-  </si>
-  <si>
-    <t>ADAMS, DANY</t>
-  </si>
-  <si>
-    <t>AIKENS, KRISTINA</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
+  <fonts count="1">
     <font>
-      <sz val="12"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="12"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -71,24 +43,15 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
 </styleSheet>
 </file>
 
@@ -388,47 +351,83 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="10.625" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="32.875" bestFit="1" customWidth="1"/>
+    <col bestFit="1" customWidth="1" max="1" min="1" width="32.875"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>full_name</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>directory_result</t>
+        </is>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>2</v>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>ABOWD, THOMAS</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Thomas Abowd</t>
+        </is>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>3</v>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>ABRAMS, DANIELLE</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Danielle Abrams</t>
+        </is>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>4</v>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>ADAMS, DANY</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Dany Adams, Ph.D.</t>
+        </is>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>5</v>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>AIKENS, KRISTINA</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Kristina Aikens, PhD</t>
+        </is>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
</xml_diff>